<commit_message>
cập nhật kết ủa sáng 11-7
</commit_message>
<xml_diff>
--- a/Relax.xlsx
+++ b/Relax.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D53182-7257-4CA1-AA9D-48A51B0BF85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92077AC-22E1-434A-B1AB-95FA519C0E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="15" windowWidth="20370" windowHeight="10905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KeHoach" sheetId="5" r:id="rId1"/>
@@ -2344,7 +2344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2200" uniqueCount="1299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="1299">
   <si>
     <t>https://www.youtube.com/watch?v=T77wtm-2exE</t>
   </si>
@@ -11693,7 +11693,7 @@
   <dimension ref="A1:AB284"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11776,7 +11776,7 @@
       </c>
       <c r="N2" s="15">
         <f>PS!M2+SUM(D:D)-SUM(O2:Q2)</f>
-        <v>55025.942279999988</v>
+        <v>55115.442279999988</v>
       </c>
       <c r="O2" s="15">
         <v>62924</v>
@@ -11925,7 +11925,7 @@
       </c>
       <c r="N6" s="21">
         <f ca="1">-N9+0*J86+PS!M6*0+N12+J77+J73+J75+5080+J71+J69+J67+J65+J63+J61+J59+J56+J54+J48+J50+J52+J46+J44+J42+J40+J38+8230+J36+J35+J33+J34+J27+J32+J31+J30+J29+J26+J24+J22+1000+J20+J10+J16+J14+J12</f>
-        <v>-60321.046583332754</v>
+        <v>-60046.384083332756</v>
       </c>
       <c r="O6" s="21">
         <f>-O9+1*J86+29000-16000-800-22000-500-2200+7900+9200+4700+1000+500+7900+J135+J133+J131+11000+J127+J129+J125+J123+J121+J119+J117+J115+J113+J111+274+J110-5000+J108+J106+J102+J104+I105+1850+J100+J98+J96+J94+J93+J91+J89+J88+J84</f>
@@ -11962,7 +11962,7 @@
       </c>
       <c r="N7" s="36">
         <f ca="1">SUM(N4:N6)</f>
-        <v>234425.75663781556</v>
+        <v>234700.41913781557</v>
       </c>
       <c r="O7" s="36">
         <f>SUM(O4:O6)</f>
@@ -11995,7 +11995,7 @@
       </c>
       <c r="N8" s="65">
         <f ca="1">ROUNDDOWN((N6/(N4+N5)),3)</f>
-        <v>-0.20399999999999999</v>
+        <v>-0.20300000000000001</v>
       </c>
       <c r="O8" s="65">
         <f>ROUNDDOWN((O6/(O4+O5)),3)</f>
@@ -12061,7 +12061,7 @@
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="43">
         <f ca="1">TODAY()</f>
-        <v>44750</v>
+        <v>44753</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>90</v>
@@ -12082,15 +12082,15 @@
       <c r="G10" s="14"/>
       <c r="H10" s="97">
         <f ca="1">Table1[[#This Row],[Result]]/(E11*F11)</f>
-        <v>-0.16093071190327288</v>
+        <v>-0.15921299770690014</v>
       </c>
       <c r="I10" s="69">
         <f ca="1">Table1[[#This Row],[Date]]-A11</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J10" s="162">
         <f ca="1">-Table1[[#This Row],[Price]]*Table1[[#This Row],[Volume]]-E11*F11-Table1[[#This Row],[Commission]]-D11+I11</f>
-        <v>-25732.820833333331</v>
+        <v>-25458.158333333333</v>
       </c>
       <c r="K10" s="121" t="s">
         <v>1272</v>
@@ -12142,7 +12142,7 @@
       <c r="H11" s="97"/>
       <c r="I11" s="67">
         <f ca="1">-105/360*(I10+1)*Table1[[#This Row],[Notes]]</f>
-        <v>1739.5291666666667</v>
+        <v>2014.1916666666666</v>
       </c>
       <c r="J11" s="98">
         <f>Table1[[#This Row],[Volume]]*Table1[[#This Row],[Price]]</f>
@@ -23378,8 +23378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CE18B9-1E5D-4C51-9D03-C69B0DC41E11}">
   <dimension ref="A1:AE59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23470,7 +23470,7 @@
       </c>
       <c r="M2" s="15">
         <f>SUM(Table6[[#All],[Commission]])</f>
-        <v>18818.300000000003</v>
+        <v>18907.800000000003</v>
       </c>
       <c r="P2" t="s">
         <v>1022</v>
@@ -23609,7 +23609,7 @@
       </c>
       <c r="M5" s="21">
         <f>SUM(G:G)-M3-U5</f>
-        <v>-6983.7999999996464</v>
+        <v>-1673.2999999996391</v>
       </c>
       <c r="T5" s="160" t="s">
         <v>1223</v>
@@ -23657,7 +23657,7 @@
       </c>
       <c r="M6" s="21">
         <f>-M3-M2+SUM(Table6[[#All],[Vị thế đóng]])-M7</f>
-        <v>30742.200000000354</v>
+        <v>36052.700000000354</v>
       </c>
       <c r="O6" s="134" t="s">
         <v>987</v>
@@ -23754,7 +23754,7 @@
       </c>
       <c r="M8" s="65">
         <f>ROUNDDOWN((M6/(M4)),3)</f>
-        <v>4.9000000000000002E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="O8" s="140" t="s">
         <v>976</v>
@@ -24280,22 +24280,29 @@
       <c r="A22" s="43">
         <v>44753</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="16"/>
+      <c r="B22" s="14" t="s">
+        <v>825</v>
+      </c>
+      <c r="C22" s="16">
+        <f>89.5</f>
+        <v>89.5</v>
+      </c>
       <c r="D22" s="14">
         <v>1225</v>
       </c>
       <c r="E22" s="14">
         <v>10</v>
       </c>
-      <c r="F22" s="98"/>
+      <c r="F22" s="98">
+        <v>5400</v>
+      </c>
       <c r="G22" s="153">
         <f>Table6[[#This Row],[Vị thế đóng]]-Table6[[#This Row],[Commission]]</f>
-        <v>0</v>
+        <v>5310.5</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="152">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="J22" s="45" t="s">
         <v>1298</v>

</xml_diff>

<commit_message>
update 19-7-22 san luong
</commit_message>
<xml_diff>
--- a/Relax.xlsx
+++ b/Relax.xlsx
@@ -2343,7 +2343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2221" uniqueCount="1310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2225" uniqueCount="1312">
   <si>
     <t>https://www.youtube.com/watch?v=T77wtm-2exE</t>
   </si>
@@ -7223,6 +7223,12 @@
   </si>
   <si>
     <t xml:space="preserve">Định vào lệnh ATO và chốt lệnh ATC, nhưng mở phiên đã xuất hiện GAP tăng lên 1219 nên quyết định đứng ngoài để mua được giá tốt hơn và chốt lệnh trong ATC hoặc giữ qua tuần đều đc =&gt; sai lầm khi không chốt lời như mọi khi 2,3 giá, để giờ lỗ gần 7 giá và quyết định giữ sang tuần vì dự báo không có gì xấu - thứ 2 nạp tiền vào giữ lệnh - chấp nhận lỗ 20 giá </t>
+  </si>
+  <si>
+    <t>giữ lệnh từ thứ 6, có cơ hội chốt lời mà ko chốt</t>
+  </si>
+  <si>
+    <t>Ngày đáo hạn PS, coi mấy ảnh diễn trò</t>
   </si>
 </sst>
 </file>
@@ -11699,8 +11705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="A9:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11783,7 +11789,7 @@
       </c>
       <c r="N2" s="15">
         <f>PS!M2+SUM(D:D)-SUM(O2:Q2)</f>
-        <v>56605.442279999988</v>
+        <v>56766.692279999988</v>
       </c>
       <c r="O2" s="15">
         <v>62924</v>
@@ -11932,7 +11938,7 @@
       </c>
       <c r="N6" s="21">
         <f ca="1">-N9+0*J88+PS!M6*0+N12+J79+J75+J77+5080+J73+J71+J69+J67+J65+J63+J61+J58+J56+J50+J52+J54+J48+J46+J44+J42+J40+8230+J38+J37+J35+J36+J29+J34+J33+J32+J31+J28+J26+J24+1000+J22+J10+J18+J16+J14+J12</f>
-        <v>-31885.50491666609</v>
+        <v>-26484.742416666086</v>
       </c>
       <c r="O6" s="21">
         <f>-O9+1*J88+29000-16000-800-22000-500-2200+7900+9200+4700+1000+500+7900+J137+J135+J133+11000+J129+J131+J127+J125+J123+J121+J119+J117+J115+J113+274+J112-5000+J110+J108+J104+J106+I107+1850+J102+J100+J98+J96+J95+J93+J91+J90+J86</f>
@@ -11969,7 +11975,7 @@
       </c>
       <c r="N7" s="36">
         <f ca="1">SUM(N4:N6)</f>
-        <v>408861.29830448225</v>
+        <v>414262.06080448226</v>
       </c>
       <c r="O7" s="36">
         <f>SUM(O4:O6)</f>
@@ -12009,7 +12015,7 @@
       </c>
       <c r="N8" s="65">
         <f ca="1">ROUNDDOWN((N6/(N4+N5)),3)</f>
-        <v>-7.1999999999999995E-2</v>
+        <v>-0.06</v>
       </c>
       <c r="O8" s="65">
         <f>ROUNDDOWN((O6/(O4+O5)),3)</f>
@@ -12085,10 +12091,10 @@
       </c>
       <c r="D10" s="16">
         <f>-F10*E10*0.0025</f>
-        <v>363.75</v>
+        <v>372.5</v>
       </c>
       <c r="E10" s="14">
-        <v>14.55</v>
+        <v>14.9</v>
       </c>
       <c r="F10" s="14">
         <v>-10000</v>
@@ -12096,7 +12102,7 @@
       <c r="G10" s="14"/>
       <c r="H10" s="97">
         <f ca="1">Table1[[#This Row],[Result]]/(E11*F11)</f>
-        <v>-7.7226573900354395E-2</v>
+        <v>-7.4642067959141134E-2</v>
       </c>
       <c r="I10" s="69">
         <f ca="1">Table1[[#This Row],[Date]]-A11</f>
@@ -12104,7 +12110,7 @@
       </c>
       <c r="J10" s="162">
         <f ca="1">-Table1[[#This Row],[Price]]*Table1[[#This Row],[Volume]]-E11*F11-Table1[[#This Row],[Commission]]-D11+I11</f>
-        <v>-12348.529166666667</v>
+        <v>-11935.266666666666</v>
       </c>
       <c r="K10" s="121" t="s">
         <v>1272</v>
@@ -12156,15 +12162,14 @@
       <c r="H11" s="97"/>
       <c r="I11" s="67">
         <f ca="1">-105/360*(I10+1)*Table1[[#This Row],[Notes]]</f>
-        <v>2655.0708333333332</v>
+        <v>-422.91666666666669</v>
       </c>
       <c r="J11" s="98">
         <f>Table1[[#This Row],[Volume]]*Table1[[#This Row],[Price]]</f>
         <v>159900</v>
       </c>
       <c r="K11" s="109">
-        <f>Table1[[#This Row],[Result]]/1000-(446+8.8+7+12)</f>
-        <v>-313.89999999999998</v>
+        <v>50</v>
       </c>
       <c r="L11" t="s">
         <v>756</v>
@@ -12201,10 +12206,10 @@
       </c>
       <c r="D12" s="16">
         <f>-F12*E12*0.0025</f>
-        <v>732.5</v>
+        <v>745</v>
       </c>
       <c r="E12" s="14">
-        <v>14.65</v>
+        <v>14.9</v>
       </c>
       <c r="F12" s="14">
         <v>-20000</v>
@@ -12212,7 +12217,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="97">
         <f>Table1[[#This Row],[Result]]/(E13*F13)</f>
-        <v>5.4238738738738738E-2</v>
+        <v>7.2211711711711715E-2</v>
       </c>
       <c r="I12" s="69">
         <f ca="1">Table1[[#This Row],[Date]]-A13</f>
@@ -12220,7 +12225,7 @@
       </c>
       <c r="J12" s="162">
         <f>-Table1[[#This Row],[Price]]*Table1[[#This Row],[Volume]]-E13*F13-Table1[[#This Row],[Commission]]-D13+I13</f>
-        <v>15051.25</v>
+        <v>20038.75</v>
       </c>
       <c r="K12" s="121" t="s">
         <v>1300</v>
@@ -23470,8 +23475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE59"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23562,7 +23567,7 @@
       </c>
       <c r="M2" s="15">
         <f>SUM(Table6[[#All],[Commission]])</f>
-        <v>19217.800000000003</v>
+        <v>19357.800000000003</v>
       </c>
       <c r="P2" t="s">
         <v>1022</v>
@@ -23701,7 +23706,7 @@
       </c>
       <c r="M5" s="21">
         <f>SUM(G:G)-M3-U5</f>
-        <v>-10544.299999999646</v>
+        <v>-2034.2999999996391</v>
       </c>
       <c r="T5" s="160" t="s">
         <v>1223</v>
@@ -23749,7 +23754,7 @@
       </c>
       <c r="M6" s="21">
         <f>-M3-M2+SUM(Table6[[#All],[Vị thế đóng]])-M7</f>
-        <v>27181.700000000354</v>
+        <v>35691.700000000354</v>
       </c>
       <c r="O6" s="134" t="s">
         <v>987</v>
@@ -23846,7 +23851,7 @@
       </c>
       <c r="M8" s="65">
         <f>ROUNDDOWN((M6/(M4)),3)</f>
-        <v>4.2999999999999997E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="O8" s="140" t="s">
         <v>976</v>
@@ -24153,7 +24158,9 @@
       </c>
       <c r="H15" s="24"/>
       <c r="I15" s="152"/>
-      <c r="J15" s="45"/>
+      <c r="J15" s="45" t="s">
+        <v>1311</v>
+      </c>
       <c r="L15" t="s">
         <v>1307</v>
       </c>
@@ -24174,7 +24181,9 @@
       <c r="A16" s="43">
         <v>44761</v>
       </c>
-      <c r="B16" s="14"/>
+      <c r="B16" s="14" t="s">
+        <v>969</v>
+      </c>
       <c r="C16" s="16"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -24203,18 +24212,31 @@
       <c r="A17" s="43">
         <v>44760</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="98"/>
+      <c r="B17" s="14" t="s">
+        <v>969</v>
+      </c>
+      <c r="C17" s="16">
+        <v>140</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1210.0999999999999</v>
+      </c>
+      <c r="E17" s="14">
+        <v>5</v>
+      </c>
+      <c r="F17" s="98">
+        <f>(15.4-10.1)*500</f>
+        <v>2650.0000000000005</v>
+      </c>
       <c r="G17" s="153">
         <f>Table6[[#This Row],[Vị thế đóng]]-Table6[[#This Row],[Commission]]</f>
-        <v>0</v>
+        <v>2510.0000000000005</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="152"/>
-      <c r="J17" s="45"/>
+      <c r="J17" s="45" t="s">
+        <v>1310</v>
+      </c>
       <c r="L17" t="s">
         <v>1296</v>
       </c>
@@ -24245,11 +24267,11 @@
         <v>5</v>
       </c>
       <c r="F18" s="98">
-        <v>-10000</v>
+        <v>-4000</v>
       </c>
       <c r="G18" s="153">
         <f>Table6[[#This Row],[Vị thế đóng]]-Table6[[#This Row],[Commission]]</f>
-        <v>-10155</v>
+        <v>-4155</v>
       </c>
       <c r="H18" s="24"/>
       <c r="I18" s="152">

</xml_diff>